<commit_message>
Agregada formulas A excel deberia ayudar
esta llena de ciclos anidados
</commit_message>
<xml_diff>
--- a/UInfo.xlsx
+++ b/UInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Proyecto final AHK\Proyecto_Tabletop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E451010A-1F20-4142-B275-9487C2193A83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBADB25-6E70-4B88-904C-BC15F582044E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E0F27C7E-EA54-46D9-90DC-7741199197B8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>X</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>Estas serian las celdas que cuentan como interacciones</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>steps</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -440,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432669D6-37ED-45C1-AD7A-B2DF266F73F3}">
-  <dimension ref="B4:H6"/>
+  <dimension ref="B2:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,15 +460,56 @@
     <col min="1" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1">
+        <f>H4</f>
+        <v>132</v>
+      </c>
+    </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="C4" s="2">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <f>IF(C3&gt;=1,C4+D3)</f>
+        <v>32</v>
+      </c>
+      <c r="E4" s="2">
+        <f>IF(C3&gt;=2,D4+D3)</f>
+        <v>57</v>
+      </c>
+      <c r="F4" s="2">
+        <f>IF(C3&gt;=3,E4+D3)</f>
+        <v>82</v>
+      </c>
+      <c r="G4" s="2">
+        <f>IF(C3&gt;=4,F4+D3)</f>
+        <v>107</v>
+      </c>
+      <c r="H4" s="2">
+        <f>IF(C3&gt;=5,G4+D3)</f>
+        <v>132</v>
+      </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -470,6 +520,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D6" s="3" t="s">
@@ -486,5 +537,8 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <cellWatches>
+    <cellWatch r="E4"/>
+  </cellWatches>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualizacion de formulas para integrales
</commit_message>
<xml_diff>
--- a/UInfo.xlsx
+++ b/UInfo.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Proyecto final AHK\Proyecto_Tabletop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBADB25-6E70-4B88-904C-BC15F582044E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB4D3E1-CB13-432E-8D79-AA18648BB0B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E0F27C7E-EA54-46D9-90DC-7741199197B8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>X</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
@@ -449,10 +455,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432669D6-37ED-45C1-AD7A-B2DF266F73F3}">
-  <dimension ref="B2:H6"/>
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="B2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +467,7 @@
     <col min="1" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -471,7 +478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C3" s="1">
         <v>5</v>
       </c>
@@ -483,7 +490,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -511,7 +518,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -522,7 +529,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D6" s="3" t="s">
         <v>2</v>
       </c>
@@ -530,6 +537,20 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="b">
+        <f>IF(MOD(C3,2)=0,(F3/3)*C5+(4*D5)+(4*E5)+(4*F5)+(4*G5)+H5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
segundo xlsx y mejora del programa
</commit_message>
<xml_diff>
--- a/UInfo.xlsx
+++ b/UInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Proyecto final AHK\Proyecto_Tabletop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB4D3E1-CB13-432E-8D79-AA18648BB0B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEF8752-3CFD-4E93-9F0A-F66D98E0163D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E0F27C7E-EA54-46D9-90DC-7741199197B8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>X</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Estas serian las celdas que cuentan como interacciones</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -55,6 +52,12 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Estas serian las celdas que cuentan como interacciones par</t>
   </si>
 </sst>
 </file>
@@ -456,105 +459,226 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432669D6-37ED-45C1-AD7A-B2DF266F73F3}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="B2:I15"/>
+  <dimension ref="B2:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="2" width="11.5546875" style="1"/>
+    <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="1" customWidth="1"/>
+    <col min="5" max="7" width="11.5546875" style="1"/>
+    <col min="8" max="8" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1">
-        <v>25</v>
+        <v>0.25</v>
       </c>
       <c r="E3" s="1">
-        <f>H4</f>
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>(E3-C4)/2</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
-        <f>IF(C3&gt;=1,C4+D3)</f>
-        <v>32</v>
+        <f>IF(C3&gt;=1,C4+D3,"")</f>
+        <v>1.25</v>
       </c>
       <c r="E4" s="2">
-        <f>IF(C3&gt;=2,D4+D3)</f>
-        <v>57</v>
+        <f>IF(C3&gt;=2,D4+D3,"")</f>
+        <v>1.5</v>
       </c>
       <c r="F4" s="2">
-        <f>IF(C3&gt;=3,E4+D3)</f>
-        <v>82</v>
+        <f>IF(C3&gt;=3,E4+D3,"")</f>
+        <v>1.75</v>
       </c>
       <c r="G4" s="2">
-        <f>IF(C3&gt;=4,F4+D3)</f>
-        <v>107</v>
-      </c>
-      <c r="H4" s="2">
-        <f>IF(C3&gt;=5,G4+D3)</f>
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+        <f>IF(C3&gt;=4,F4+D3,"")</f>
+        <v>2</v>
+      </c>
+      <c r="H4" s="2" t="str">
+        <f>IF(C3&gt;=5,G4+D3,"")</f>
+        <v/>
+      </c>
+      <c r="I4" s="2" t="str">
+        <f>IF(C3&gt;=6,H4+D3,"")</f>
+        <v/>
+      </c>
+      <c r="J4" s="2" t="str">
+        <f>IF(C3&gt;=7,I4+D3,"")</f>
+        <v/>
+      </c>
+      <c r="K4" s="2" t="str">
+        <f>IF(C3&gt;=8,J4+D3,"")</f>
+        <v/>
+      </c>
+      <c r="L4" s="2" t="str">
+        <f>IF(C3&gt;=9,K4+D3,"")</f>
+        <v/>
+      </c>
+      <c r="M4" s="2" t="str">
+        <f>IF(C3&gt;=10,L4+D3,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E8" s="1" t="b">
-        <f>IF(MOD(C3,2)=0,(F3/3)*C5+(4*D5)+(4*E5)+(4*F5)+(4*G5)+H5)</f>
+      <c r="C5" s="2">
+        <f>(((2*C4)+1)*(C4-2)/C4)</f>
+        <v>-3</v>
+      </c>
+      <c r="D5" s="2">
+        <f>IF(D4="","",(((2*D4)+1)*((D4-2))/D4))</f>
+        <v>-2.1</v>
+      </c>
+      <c r="E5" s="2">
+        <f>IF(E4="","",(((2*E4)+1)*(E4-2)/E4))</f>
+        <v>-1.3333333333333333</v>
+      </c>
+      <c r="F5" s="2">
+        <f>IF(F4="","",(((2*F4)+1)*(F4-2)/F4))</f>
+        <v>-0.6428571428571429</v>
+      </c>
+      <c r="G5" s="2">
+        <f>IF(G4="","",(((2*G4)+1)*(G4-2)/G4))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="1" t="s">
+      <c r="H5" s="2" t="str">
+        <f t="shared" ref="E5:K5" si="0">IF(H4="","",1)</f>
+        <v/>
+      </c>
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L5" s="2" t="str">
+        <f>IF(L4="","",1)</f>
+        <v/>
+      </c>
+      <c r="M5" s="2" t="str">
+        <f>IF(M4="","",1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="1">
+        <f>IF(OR(E5="",C3=1),IF(AND(E5="",C3=1),1,0),IF(C3=2,4,1))</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <f>IF(OR(F5="",C3=2),IF(AND(F5="",C3=2),1,0),IF(C3=4,4,1))</f>
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <f>IF(OR(G5="",C3=3),IF(AND(G5="",C3=3),1,0),IF(C3=6,4,1))</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <f>IF(OR(H5="",C3=4),IF(AND(H5="",C3=4),1,0),IF(C3=8,4,1))</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <f>IF(OR(I5="",C3=5),IF(AND(I5="",C3=5),1,0),IF(C3=10,4,1))</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <f>IF(OR(J5="",C3=6),IF(AND(J5="",C3=6),1,0),1)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <f>IF(OR(K5="",C3=7),IF(AND(K5="",C3=7),1,0),1)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <f>IF(OR(L5="",C3=8),IF(AND(L5="",C3=8),1,0),1)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <f>IF(OR(M5="",C3=9),IF(AND(M5="",C3=9),1,0),1)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <f>(F3/3)*(C5+IF(D4="",0,IF(C3=2,(D5*D6),0))+IF(E4="",0,IF(C3=4,(E5*E6),IF(C3=2,E5)))+IF(F4="",0,IF(C3=6,(F5*F6),0)+IF(G4="",0,IF(C3=8,(G5*G6),IF(C3=4,G5)+IF(H4="",0,IF(C3=10,(H5*H6),0)+IF(I4="",0,IF(C3=6,(I5*I6)))+IF(J4="",0,IF(C3=8,(J5*J6)))+IF(K4="",0,IF(C3=10,(K5*K6)))+IF(L4="",0,(L5*L6))+IF(M4="",0,(M5*M6)))))))</f>
+        <v>-1.3888888888888886</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H11" s="1">
+        <f>X2+4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H12" s="1" t="str">
+        <f>SUBSTITUTE(H11,"x",D4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="K8:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
se movio el cuadro de la primera Sprdshe, no acomodaba con las demas
</commit_message>
<xml_diff>
--- a/UInfo.xlsx
+++ b/UInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Proyecto final AHK\Proyecto_Tabletop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97EBD82-EE3B-49AC-9CA5-13E791A5D419}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB932B15-627B-453E-BBE9-2530826C8B5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MetodoTrapecio" sheetId="1" r:id="rId1"/>
@@ -1248,7 +1248,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1285,7 +1285,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-PA"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1449,7 +1449,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-PA"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1581,7 +1581,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-PA"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="513646600"/>
@@ -1643,7 +1643,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-PA"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="513645944"/>
@@ -1691,7 +1691,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PA"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1705,7 +1705,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1742,7 +1742,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-PA"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1878,7 +1878,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-PA"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1998,7 +1998,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-PA"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="602881984"/>
@@ -2060,7 +2060,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-PA"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="602883952"/>
@@ -2101,7 +2101,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PA"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3307,7 +3307,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3605,11 +3605,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView zoomScale="83" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.44140625" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" customWidth="1"/>
@@ -3839,11 +3839,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FE13D7-10D2-4046-AC07-C92F376A534D}">
   <dimension ref="A2:L36"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.44140625" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" customWidth="1"/>
@@ -4110,11 +4110,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A119582-7117-47F0-AF1E-35CC75B347B9}">
   <dimension ref="A2:L44"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25.88671875" customWidth="1"/>
     <col min="3" max="3" width="26.44140625" customWidth="1"/>
@@ -4452,7 +4452,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25.88671875" customWidth="1"/>
     <col min="3" max="3" width="26.44140625" customWidth="1"/>
@@ -4729,7 +4729,7 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.21875" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" customWidth="1"/>

</xml_diff>